<commit_message>
Cost Center Negative Test cases added
</commit_message>
<xml_diff>
--- a/tests/artifact/script/CostCenter.xlsx
+++ b/tests/artifact/script/CostCenter.xlsx
@@ -2315,7 +2315,7 @@
 password=${password}</t>
   </si>
   <si>
-    <t>Edit Product Details</t>
+    <t>Cost Centre and Cost center Statment Test cases</t>
   </si>
   <si>
     <t>Go to Cost Center page</t>
@@ -9618,8 +9618,8 @@
   <sheetPr/>
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
chnages in teh file
</commit_message>
<xml_diff>
--- a/tests/artifact/script/CostCenter.xlsx
+++ b/tests/artifact/script/CostCenter.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Login" sheetId="10" r:id="rId2"/>
-    <sheet name="CostCenter" sheetId="11" r:id="rId3"/>
+    <sheet name="Positive-CostCenter" sheetId="11" r:id="rId3"/>
+    <sheet name="Negative-CostCenter" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="844">
   <si>
     <t>target</t>
   </si>
@@ -9618,8 +9619,8 @@
   <sheetPr/>
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -9691,7 +9692,7 @@
       <c r="N2" s="53"/>
       <c r="O2" s="53"/>
     </row>
-    <row r="3" s="2" customFormat="1" ht="10" customHeight="1" spans="1:15">
+    <row r="3" s="2" customFormat="1" ht="15.15" spans="1:15">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
@@ -9708,7 +9709,7 @@
       <c r="N3" s="26"/>
       <c r="O3" s="25"/>
     </row>
-    <row r="4" s="3" customFormat="1" ht="24" customHeight="1" spans="1:15">
+    <row r="4" s="3" customFormat="1" ht="15.15" spans="1:15">
       <c r="A4" s="27" t="s">
         <v>733</v>
       </c>
@@ -9753,7 +9754,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="1" ht="26" customHeight="1" spans="1:15">
+    <row r="5" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A5" s="22" t="s">
         <v>751</v>
       </c>
@@ -9782,7 +9783,7 @@
       <c r="N5" s="26"/>
       <c r="O5" s="25"/>
     </row>
-    <row r="6" s="4" customFormat="1" ht="22" customHeight="1" spans="1:15">
+    <row r="6" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A6" s="22"/>
       <c r="B6" s="23" t="s">
         <v>754</v>
@@ -9809,7 +9810,7 @@
       <c r="N6" s="26"/>
       <c r="O6" s="25"/>
     </row>
-    <row r="7" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
+    <row r="7" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A7" s="22"/>
       <c r="B7" s="23" t="s">
         <v>756</v>
@@ -9836,7 +9837,7 @@
       <c r="N7" s="26"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
+    <row r="8" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A8" s="22"/>
       <c r="B8" s="23" t="s">
         <v>758</v>
@@ -9863,7 +9864,7 @@
       <c r="N8" s="26"/>
       <c r="O8" s="25"/>
     </row>
-    <row r="9" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="9" s="5" customFormat="1" spans="1:15">
       <c r="A9" s="31"/>
       <c r="B9" s="23" t="s">
         <v>760</v>
@@ -9890,7 +9891,7 @@
       <c r="N9" s="59"/>
       <c r="O9" s="58"/>
     </row>
-    <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="10" s="2" customFormat="1" spans="1:15">
       <c r="A10" s="22" t="s">
         <v>762</v>
       </c>
@@ -9919,7 +9920,7 @@
       <c r="N10" s="26"/>
       <c r="O10" s="25"/>
     </row>
-    <row r="11" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="11" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A11" s="22"/>
       <c r="B11" s="23" t="s">
         <v>766</v>
@@ -9944,7 +9945,7 @@
       <c r="N11" s="26"/>
       <c r="O11" s="25"/>
     </row>
-    <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="12" s="2" customFormat="1" spans="1:15">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>768</v>
@@ -9971,7 +9972,7 @@
       <c r="N12" s="26"/>
       <c r="O12" s="25"/>
     </row>
-    <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="13" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>771</v>
@@ -9996,7 +9997,7 @@
       <c r="N13" s="26"/>
       <c r="O13" s="25"/>
     </row>
-    <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="14" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A14" s="22"/>
       <c r="B14" s="23" t="s">
         <v>773</v>
@@ -10023,7 +10024,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="25"/>
     </row>
-    <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="15" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A15" s="22"/>
       <c r="B15" s="23" t="s">
         <v>776</v>
@@ -10048,7 +10049,7 @@
       <c r="N15" s="26"/>
       <c r="O15" s="25"/>
     </row>
-    <row r="16" s="4" customFormat="1" ht="22" customHeight="1" spans="1:7">
+    <row r="16" s="4" customFormat="1" ht="15.6" spans="1:7">
       <c r="A16" s="22"/>
       <c r="B16" s="23" t="s">
         <v>778</v>
@@ -10067,7 +10068,7 @@
       </c>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="17" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A17" s="22" t="s">
         <v>780</v>
       </c>
@@ -10096,7 +10097,7 @@
       <c r="N17" s="26"/>
       <c r="O17" s="25"/>
     </row>
-    <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="18" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A18" s="22"/>
       <c r="B18" s="23" t="s">
         <v>783</v>
@@ -10123,7 +10124,7 @@
       <c r="N18" s="26"/>
       <c r="O18" s="25"/>
     </row>
-    <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="19" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A19" s="22"/>
       <c r="B19" s="23" t="s">
         <v>784</v>
@@ -10148,7 +10149,7 @@
       <c r="N19" s="26"/>
       <c r="O19" s="25"/>
     </row>
-    <row r="20" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="20" s="2" customFormat="1" spans="1:15">
       <c r="A20" s="22"/>
       <c r="B20" s="23" t="s">
         <v>785</v>
@@ -10173,7 +10174,7 @@
       <c r="N20" s="26"/>
       <c r="O20" s="25"/>
     </row>
-    <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="21" s="2" customFormat="1" spans="1:15">
       <c r="A21" s="22"/>
       <c r="B21" s="23" t="s">
         <v>787</v>
@@ -10198,7 +10199,7 @@
       <c r="N21" s="26"/>
       <c r="O21" s="25"/>
     </row>
-    <row r="22" s="4" customFormat="1" ht="22" customHeight="1" spans="1:7">
+    <row r="22" s="4" customFormat="1" ht="15.6" spans="1:7">
       <c r="A22" s="22" t="s">
         <v>789</v>
       </c>
@@ -10217,7 +10218,7 @@
       <c r="F22" s="39"/>
       <c r="G22" s="29"/>
     </row>
-    <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="23" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A23" s="22"/>
       <c r="B23" s="23" t="s">
         <v>792</v>
@@ -10244,7 +10245,7 @@
       <c r="N23" s="26"/>
       <c r="O23" s="25"/>
     </row>
-    <row r="24" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="24" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A24" s="22"/>
       <c r="B24" s="23" t="s">
         <v>794</v>
@@ -10271,7 +10272,7 @@
       <c r="N24" s="26"/>
       <c r="O24" s="25"/>
     </row>
-    <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="25" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A25" s="22"/>
       <c r="B25" s="23" t="s">
         <v>795</v>
@@ -10296,7 +10297,7 @@
       <c r="N25" s="26"/>
       <c r="O25" s="25"/>
     </row>
-    <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="26" s="2" customFormat="1" spans="1:15">
       <c r="A26" s="22"/>
       <c r="B26" s="23" t="s">
         <v>785</v>
@@ -10321,7 +10322,7 @@
       <c r="N26" s="26"/>
       <c r="O26" s="25"/>
     </row>
-    <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="27" s="2" customFormat="1" spans="1:15">
       <c r="A27" s="22"/>
       <c r="B27" s="23" t="s">
         <v>787</v>
@@ -10346,7 +10347,7 @@
       <c r="N27" s="26"/>
       <c r="O27" s="25"/>
     </row>
-    <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="28" s="2" customFormat="1" spans="1:15">
       <c r="A28" s="22" t="s">
         <v>797</v>
       </c>
@@ -10373,7 +10374,7 @@
       <c r="N28" s="26"/>
       <c r="O28" s="25"/>
     </row>
-    <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="29" s="2" customFormat="1" spans="1:15">
       <c r="A29" s="22"/>
       <c r="B29" s="23" t="s">
         <v>800</v>
@@ -10398,7 +10399,7 @@
       <c r="N29" s="26"/>
       <c r="O29" s="25"/>
     </row>
-    <row r="30" s="2" customFormat="1" ht="31" customHeight="1" spans="1:15">
+    <row r="30" s="2" customFormat="1" spans="1:15">
       <c r="A30" s="22"/>
       <c r="B30" s="23" t="s">
         <v>802</v>
@@ -10423,7 +10424,7 @@
       <c r="N30" s="26"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" s="2" customFormat="1" ht="31" customHeight="1" spans="1:15">
+    <row r="31" s="2" customFormat="1" spans="1:15">
       <c r="A31" s="22"/>
       <c r="B31" s="23" t="s">
         <v>804</v>
@@ -10448,7 +10449,7 @@
       <c r="N31" s="26"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" s="2" customFormat="1" ht="31" customHeight="1" spans="1:15">
+    <row r="32" s="2" customFormat="1" spans="1:15">
       <c r="A32" s="22"/>
       <c r="B32" s="23" t="s">
         <v>806</v>
@@ -10473,7 +10474,7 @@
       <c r="N32" s="26"/>
       <c r="O32" s="25"/>
     </row>
-    <row r="33" s="2" customFormat="1" ht="31" customHeight="1" spans="1:15">
+    <row r="33" s="2" customFormat="1" spans="1:15">
       <c r="A33" s="22"/>
       <c r="B33" s="23" t="s">
         <v>808</v>
@@ -10498,7 +10499,7 @@
       <c r="N33" s="26"/>
       <c r="O33" s="25"/>
     </row>
-    <row r="34" s="2" customFormat="1" ht="31" customHeight="1" spans="1:15">
+    <row r="34" s="2" customFormat="1" spans="1:15">
       <c r="A34" s="22"/>
       <c r="B34" s="23" t="s">
         <v>810</v>
@@ -10523,7 +10524,7 @@
       <c r="N34" s="26"/>
       <c r="O34" s="25"/>
     </row>
-    <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="35" s="2" customFormat="1" spans="1:15">
       <c r="A35" s="22"/>
       <c r="B35" s="23" t="s">
         <v>812</v>
@@ -10548,7 +10549,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="25"/>
     </row>
-    <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="36" s="2" customFormat="1" spans="1:15">
       <c r="A36" s="22"/>
       <c r="B36" s="23" t="s">
         <v>814</v>
@@ -10573,7 +10574,7 @@
       <c r="N36" s="26"/>
       <c r="O36" s="25"/>
     </row>
-    <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="37" s="2" customFormat="1" spans="1:15">
       <c r="A37" s="22"/>
       <c r="B37" s="23" t="s">
         <v>816</v>
@@ -10598,7 +10599,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="25"/>
     </row>
-    <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="38" s="2" customFormat="1" spans="1:15">
       <c r="A38" s="22"/>
       <c r="B38" s="23" t="s">
         <v>817</v>
@@ -10623,7 +10624,7 @@
       <c r="N38" s="26"/>
       <c r="O38" s="25"/>
     </row>
-    <row r="39" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="39" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A39" s="22" t="s">
         <v>819</v>
       </c>
@@ -10652,7 +10653,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="25"/>
     </row>
-    <row r="40" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="40" s="2" customFormat="1" ht="15.6" spans="1:15">
       <c r="A40" s="22"/>
       <c r="B40" s="23" t="s">
         <v>822</v>
@@ -10679,7 +10680,7 @@
       <c r="N40" s="26"/>
       <c r="O40" s="25"/>
     </row>
-    <row r="41" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="41" s="2" customFormat="1" spans="1:15">
       <c r="A41" s="22"/>
       <c r="B41" s="23" t="s">
         <v>825</v>
@@ -10704,7 +10705,7 @@
       <c r="N41" s="26"/>
       <c r="O41" s="25"/>
     </row>
-    <row r="42" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="42" s="2" customFormat="1" spans="1:15">
       <c r="A42" s="22" t="s">
         <v>826</v>
       </c>
@@ -10731,7 +10732,7 @@
       <c r="N42" s="26"/>
       <c r="O42" s="25"/>
     </row>
-    <row r="43" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="43" s="2" customFormat="1" spans="1:15">
       <c r="A43" s="22"/>
       <c r="B43" s="23" t="s">
         <v>829</v>
@@ -10756,7 +10757,7 @@
       <c r="N43" s="26"/>
       <c r="O43" s="25"/>
     </row>
-    <row r="44" s="2" customFormat="1" ht="21" customHeight="1" spans="1:15">
+    <row r="44" s="2" customFormat="1" spans="1:15">
       <c r="A44" s="22"/>
       <c r="B44" s="23" t="s">
         <v>831</v>
@@ -10781,7 +10782,7 @@
       <c r="N44" s="26"/>
       <c r="O44" s="25"/>
     </row>
-    <row r="45" s="2" customFormat="1" ht="27" customHeight="1" spans="1:15">
+    <row r="45" s="2" customFormat="1" spans="1:15">
       <c r="A45" s="22"/>
       <c r="B45" s="23" t="s">
         <v>833</v>
@@ -10806,7 +10807,7 @@
       <c r="N45" s="26"/>
       <c r="O45" s="25"/>
     </row>
-    <row r="46" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="46" s="2" customFormat="1" spans="1:15">
       <c r="A46" s="22"/>
       <c r="B46" s="23" t="s">
         <v>835</v>
@@ -10831,7 +10832,7 @@
       <c r="N46" s="26"/>
       <c r="O46" s="25"/>
     </row>
-    <row r="47" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="47" s="2" customFormat="1" spans="1:15">
       <c r="A47" s="22"/>
       <c r="B47" s="23" t="s">
         <v>837</v>
@@ -10856,7 +10857,7 @@
       <c r="N47" s="26"/>
       <c r="O47" s="25"/>
     </row>
-    <row r="48" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
+    <row r="48" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A48" s="22" t="s">
         <v>839</v>
       </c>
@@ -10885,7 +10886,7 @@
       <c r="N48" s="26"/>
       <c r="O48" s="25"/>
     </row>
-    <row r="49" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
+    <row r="49" s="4" customFormat="1" ht="15.6" spans="1:15">
       <c r="A49" s="22"/>
       <c r="B49" s="23" t="s">
         <v>758</v>
@@ -10912,7 +10913,7 @@
       <c r="N49" s="26"/>
       <c r="O49" s="25"/>
     </row>
-    <row r="50" s="4" customFormat="1" ht="22" customHeight="1" spans="2:7">
+    <row r="50" s="4" customFormat="1" ht="15.6" spans="2:7">
       <c r="B50" s="4" t="s">
         <v>790</v>
       </c>
@@ -10930,7 +10931,7 @@
       </c>
       <c r="G50" s="29"/>
     </row>
-    <row r="51" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="51" s="2" customFormat="1" spans="1:15">
       <c r="A51" s="22"/>
       <c r="B51" s="23" t="s">
         <v>841</v>
@@ -10955,7 +10956,7 @@
       <c r="N51" s="26"/>
       <c r="O51" s="25"/>
     </row>
-    <row r="52" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="52" s="2" customFormat="1" spans="1:15">
       <c r="A52" s="22"/>
       <c r="B52" s="23" t="s">
         <v>843</v>
@@ -10980,7 +10981,7 @@
       <c r="N52" s="26"/>
       <c r="O52" s="25"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="53" s="1" customFormat="1" spans="1:15">
       <c r="A53" s="42"/>
       <c r="B53" s="43"/>
       <c r="C53" s="44"/>
@@ -10996,7 +10997,7 @@
       <c r="N53" s="61"/>
       <c r="O53" s="49"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="54" s="1" customFormat="1" spans="1:15">
       <c r="A54" s="42"/>
       <c r="B54" s="43"/>
       <c r="C54" s="44"/>
@@ -11012,7 +11013,7 @@
       <c r="N54" s="61"/>
       <c r="O54" s="49"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="55" s="1" customFormat="1" spans="1:15">
       <c r="A55" s="42"/>
       <c r="B55" s="43"/>
       <c r="C55" s="44"/>
@@ -11028,7 +11029,7 @@
       <c r="N55" s="61"/>
       <c r="O55" s="49"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="56" s="1" customFormat="1" spans="1:15">
       <c r="A56" s="42"/>
       <c r="B56" s="43"/>
       <c r="C56" s="44"/>
@@ -11044,7 +11045,7 @@
       <c r="N56" s="61"/>
       <c r="O56" s="49"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="57" s="1" customFormat="1" spans="1:15">
       <c r="A57" s="42"/>
       <c r="B57" s="43"/>
       <c r="C57" s="44"/>
@@ -11060,7 +11061,7 @@
       <c r="N57" s="61"/>
       <c r="O57" s="49"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="58" s="1" customFormat="1" spans="1:15">
       <c r="A58" s="42"/>
       <c r="B58" s="43"/>
       <c r="C58" s="44"/>
@@ -11076,7 +11077,7 @@
       <c r="N58" s="61"/>
       <c r="O58" s="49"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="59" s="1" customFormat="1" spans="1:15">
       <c r="A59" s="42"/>
       <c r="B59" s="43"/>
       <c r="C59" s="44"/>
@@ -11093,7 +11094,7 @@
       <c r="N59" s="61"/>
       <c r="O59" s="49"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="60" s="1" customFormat="1" spans="1:15">
       <c r="A60" s="42"/>
       <c r="B60" s="43"/>
       <c r="C60" s="44"/>
@@ -11110,7 +11111,7 @@
       <c r="N60" s="61"/>
       <c r="O60" s="49"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="61" s="1" customFormat="1" spans="1:15">
       <c r="A61" s="42"/>
       <c r="B61" s="43"/>
       <c r="C61" s="44"/>
@@ -11127,7 +11128,7 @@
       <c r="N61" s="61"/>
       <c r="O61" s="49"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="62" s="1" customFormat="1" spans="1:15">
       <c r="A62" s="42"/>
       <c r="B62" s="43"/>
       <c r="C62" s="44"/>
@@ -11144,7 +11145,7 @@
       <c r="N62" s="61"/>
       <c r="O62" s="49"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="63" s="1" customFormat="1" spans="1:15">
       <c r="A63" s="42"/>
       <c r="B63" s="43"/>
       <c r="C63" s="44"/>
@@ -11161,7 +11162,7 @@
       <c r="N63" s="61"/>
       <c r="O63" s="49"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="64" s="1" customFormat="1" spans="1:15">
       <c r="A64" s="42"/>
       <c r="B64" s="43"/>
       <c r="C64" s="44"/>
@@ -11178,7 +11179,7 @@
       <c r="N64" s="61"/>
       <c r="O64" s="49"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="65" s="1" customFormat="1" spans="1:15">
       <c r="A65" s="42"/>
       <c r="B65" s="43"/>
       <c r="C65" s="44"/>
@@ -11195,7 +11196,7 @@
       <c r="N65" s="61"/>
       <c r="O65" s="49"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="66" s="1" customFormat="1" spans="1:15">
       <c r="A66" s="42"/>
       <c r="B66" s="43"/>
       <c r="C66" s="44"/>
@@ -11331,7 +11332,7 @@
       <c r="N73" s="61"/>
       <c r="O73" s="49"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="74" s="1" customFormat="1" spans="1:15">
       <c r="A74" s="42"/>
       <c r="B74" s="43"/>
       <c r="C74" s="44"/>
@@ -11348,7 +11349,7 @@
       <c r="N74" s="61"/>
       <c r="O74" s="49"/>
     </row>
-    <row r="75" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="75" s="1" customFormat="1" spans="1:15">
       <c r="A75" s="42"/>
       <c r="B75" s="43"/>
       <c r="C75" s="44"/>
@@ -11416,7 +11417,7 @@
       <c r="N78" s="61"/>
       <c r="O78" s="49"/>
     </row>
-    <row r="79" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="79" s="1" customFormat="1" spans="1:15">
       <c r="A79" s="42"/>
       <c r="B79" s="43"/>
       <c r="C79" s="44"/>
@@ -11433,7 +11434,7 @@
       <c r="N79" s="61"/>
       <c r="O79" s="49"/>
     </row>
-    <row r="80" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="80" s="1" customFormat="1" spans="1:15">
       <c r="A80" s="42"/>
       <c r="B80" s="43"/>
       <c r="C80" s="44"/>
@@ -11450,7 +11451,7 @@
       <c r="N80" s="61"/>
       <c r="O80" s="49"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="81" s="1" customFormat="1" spans="1:15">
       <c r="A81" s="42"/>
       <c r="B81" s="43"/>
       <c r="C81" s="44"/>
@@ -11467,7 +11468,7 @@
       <c r="N81" s="61"/>
       <c r="O81" s="49"/>
     </row>
-    <row r="82" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="82" s="1" customFormat="1" spans="1:15">
       <c r="A82" s="42"/>
       <c r="B82" s="43"/>
       <c r="C82" s="28"/>
@@ -11484,7 +11485,7 @@
       <c r="N82" s="61"/>
       <c r="O82" s="49"/>
     </row>
-    <row r="83" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="83" s="6" customFormat="1" spans="1:15">
       <c r="A83" s="63"/>
       <c r="B83" s="64"/>
       <c r="C83" s="65"/>
@@ -11501,7 +11502,7 @@
       <c r="N83" s="69"/>
       <c r="O83" s="68"/>
     </row>
-    <row r="84" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="84" s="6" customFormat="1" spans="1:15">
       <c r="A84" s="63"/>
       <c r="B84" s="64"/>
       <c r="C84" s="65"/>
@@ -11518,7 +11519,7 @@
       <c r="N84" s="69"/>
       <c r="O84" s="68"/>
     </row>
-    <row r="85" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="85" s="6" customFormat="1" spans="1:15">
       <c r="A85" s="63"/>
       <c r="B85" s="64"/>
       <c r="C85" s="65"/>
@@ -11535,7 +11536,7 @@
       <c r="N85" s="69"/>
       <c r="O85" s="68"/>
     </row>
-    <row r="86" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="86" s="6" customFormat="1" spans="1:15">
       <c r="A86" s="63"/>
       <c r="B86" s="64"/>
       <c r="C86" s="65"/>
@@ -11552,7 +11553,7 @@
       <c r="N86" s="69"/>
       <c r="O86" s="68"/>
     </row>
-    <row r="87" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="87" s="6" customFormat="1" spans="1:15">
       <c r="A87" s="63"/>
       <c r="B87" s="64"/>
       <c r="C87" s="65"/>
@@ -11569,7 +11570,7 @@
       <c r="N87" s="69"/>
       <c r="O87" s="68"/>
     </row>
-    <row r="88" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="88" s="1" customFormat="1" spans="1:15">
       <c r="A88" s="42"/>
       <c r="B88" s="43"/>
       <c r="C88" s="44"/>
@@ -11586,7 +11587,7 @@
       <c r="N88" s="61"/>
       <c r="O88" s="49"/>
     </row>
-    <row r="89" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="89" s="1" customFormat="1" spans="1:15">
       <c r="A89" s="42"/>
       <c r="B89" s="43"/>
       <c r="C89" s="44"/>
@@ -11603,7 +11604,7 @@
       <c r="N89" s="61"/>
       <c r="O89" s="49"/>
     </row>
-    <row r="90" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="90" s="1" customFormat="1" spans="1:15">
       <c r="A90" s="42"/>
       <c r="B90" s="43"/>
       <c r="C90" s="44"/>
@@ -11620,7 +11621,7 @@
       <c r="N90" s="61"/>
       <c r="O90" s="49"/>
     </row>
-    <row r="91" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="91" s="1" customFormat="1" spans="1:15">
       <c r="A91" s="42"/>
       <c r="B91" s="43"/>
       <c r="C91" s="44"/>
@@ -11637,7 +11638,7 @@
       <c r="N91" s="61"/>
       <c r="O91" s="49"/>
     </row>
-    <row r="92" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="92" s="1" customFormat="1" spans="1:15">
       <c r="A92" s="42"/>
       <c r="B92" s="43"/>
       <c r="C92" s="44"/>
@@ -11654,7 +11655,7 @@
       <c r="N92" s="61"/>
       <c r="O92" s="49"/>
     </row>
-    <row r="93" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="93" s="1" customFormat="1" spans="1:15">
       <c r="A93" s="42"/>
       <c r="B93" s="43"/>
       <c r="C93" s="44"/>
@@ -11671,7 +11672,7 @@
       <c r="N93" s="61"/>
       <c r="O93" s="49"/>
     </row>
-    <row r="94" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="94" s="1" customFormat="1" spans="1:15">
       <c r="A94" s="42"/>
       <c r="B94" s="43"/>
       <c r="C94" s="44"/>
@@ -11688,7 +11689,7 @@
       <c r="N94" s="61"/>
       <c r="O94" s="49"/>
     </row>
-    <row r="95" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="95" s="1" customFormat="1" spans="1:15">
       <c r="A95" s="42"/>
       <c r="B95" s="43"/>
       <c r="C95" s="44"/>
@@ -11705,7 +11706,7 @@
       <c r="N95" s="61"/>
       <c r="O95" s="49"/>
     </row>
-    <row r="96" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="96" s="1" customFormat="1" spans="1:15">
       <c r="A96" s="42"/>
       <c r="B96" s="43"/>
       <c r="C96" s="44"/>
@@ -11722,7 +11723,7 @@
       <c r="N96" s="61"/>
       <c r="O96" s="49"/>
     </row>
-    <row r="97" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="97" s="1" customFormat="1" spans="1:15">
       <c r="A97" s="42"/>
       <c r="B97" s="43"/>
       <c r="C97" s="44"/>
@@ -11739,7 +11740,7 @@
       <c r="N97" s="61"/>
       <c r="O97" s="49"/>
     </row>
-    <row r="98" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="98" s="1" customFormat="1" spans="1:15">
       <c r="A98" s="42"/>
       <c r="B98" s="43"/>
       <c r="C98" s="44"/>
@@ -11756,7 +11757,7 @@
       <c r="N98" s="61"/>
       <c r="O98" s="49"/>
     </row>
-    <row r="99" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="99" s="1" customFormat="1" spans="1:15">
       <c r="A99" s="42"/>
       <c r="B99" s="43"/>
       <c r="C99" s="44"/>
@@ -11773,7 +11774,7 @@
       <c r="N99" s="61"/>
       <c r="O99" s="49"/>
     </row>
-    <row r="100" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="100" s="1" customFormat="1" spans="1:15">
       <c r="A100" s="42"/>
       <c r="B100" s="43"/>
       <c r="C100" s="44"/>
@@ -11790,7 +11791,7 @@
       <c r="N100" s="61"/>
       <c r="O100" s="49"/>
     </row>
-    <row r="101" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="101" s="1" customFormat="1" spans="1:15">
       <c r="A101" s="42"/>
       <c r="B101" s="43"/>
       <c r="C101" s="44"/>
@@ -11807,7 +11808,7 @@
       <c r="N101" s="61"/>
       <c r="O101" s="49"/>
     </row>
-    <row r="102" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="102" s="1" customFormat="1" spans="1:15">
       <c r="A102" s="42"/>
       <c r="B102" s="43"/>
       <c r="C102" s="44"/>
@@ -11824,7 +11825,7 @@
       <c r="N102" s="61"/>
       <c r="O102" s="49"/>
     </row>
-    <row r="103" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="103" s="1" customFormat="1" spans="1:15">
       <c r="A103" s="42"/>
       <c r="B103" s="43"/>
       <c r="C103" s="44"/>
@@ -11841,7 +11842,7 @@
       <c r="N103" s="61"/>
       <c r="O103" s="49"/>
     </row>
-    <row r="104" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="104" s="1" customFormat="1" spans="1:15">
       <c r="A104" s="42"/>
       <c r="B104" s="43"/>
       <c r="C104" s="44"/>
@@ -11858,7 +11859,7 @@
       <c r="N104" s="61"/>
       <c r="O104" s="49"/>
     </row>
-    <row r="105" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="105" s="1" customFormat="1" spans="1:15">
       <c r="A105" s="42"/>
       <c r="B105" s="43"/>
       <c r="C105" s="44"/>
@@ -11875,7 +11876,7 @@
       <c r="N105" s="61"/>
       <c r="O105" s="49"/>
     </row>
-    <row r="106" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="106" s="1" customFormat="1" spans="1:15">
       <c r="A106" s="42"/>
       <c r="B106" s="43"/>
       <c r="C106" s="44"/>
@@ -12130,4 +12131,2523 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="39.75" style="7" customWidth="1"/>
+    <col min="2" max="2" width="49.625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10" style="9" customWidth="1"/>
+    <col min="4" max="4" width="47.3333333333333" style="10" customWidth="1"/>
+    <col min="5" max="5" width="70.375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="30.3333333333333" style="10" customWidth="1"/>
+    <col min="7" max="7" width="16.125" style="10" customWidth="1"/>
+    <col min="8" max="9" width="9.25" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="1.66666666666667" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12" style="13" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="14" customWidth="1"/>
+    <col min="14" max="14" width="19" style="13" customWidth="1"/>
+    <col min="15" max="15" width="49.8333333333333" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="10.8333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="15.15" spans="1:15">
+      <c r="A1" s="15" t="s">
+        <v>725</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>727</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>728</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>729</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>730</v>
+      </c>
+      <c r="J1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="17" t="s">
+        <v>731</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="50"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="15.15" spans="1:15">
+      <c r="A2" s="18" t="s">
+        <v>750</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="15.15" spans="1:15">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="25"/>
+    </row>
+    <row r="4" s="3" customFormat="1" ht="15.15" spans="1:15">
+      <c r="A4" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>725</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>734</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>735</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>736</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>737</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>738</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>740</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>741</v>
+      </c>
+      <c r="K4" s="55"/>
+      <c r="L4" s="27" t="s">
+        <v>742</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>743</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>744</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A5" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>753</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1500</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="25"/>
+    </row>
+    <row r="6" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23" t="s">
+        <v>754</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>755</v>
+      </c>
+      <c r="F6" s="30">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>756</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>757</v>
+      </c>
+      <c r="F7" s="30">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="25"/>
+    </row>
+    <row r="8" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
+        <v>758</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>759</v>
+      </c>
+      <c r="F8" s="30">
+        <v>2000</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="25"/>
+    </row>
+    <row r="9" s="5" customFormat="1" spans="1:15">
+      <c r="A9" s="31"/>
+      <c r="B9" s="23" t="s">
+        <v>760</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>761</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="58"/>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:15">
+      <c r="A10" s="22" t="s">
+        <v>762</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>763</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>764</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>765</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="25"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>767</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="25"/>
+    </row>
+    <row r="12" s="2" customFormat="1" spans="1:15">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23" t="s">
+        <v>768</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>769</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>770</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="25"/>
+    </row>
+    <row r="13" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23" t="s">
+        <v>771</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="25"/>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23" t="s">
+        <v>773</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>775</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="25"/>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23" t="s">
+        <v>776</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="25"/>
+    </row>
+    <row r="16" s="4" customFormat="1" ht="15.6" spans="1:7">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23" t="s">
+        <v>778</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>767</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>779</v>
+      </c>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A17" s="22" t="s">
+        <v>780</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>706</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>782</v>
+      </c>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>706</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="F18" s="37">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23" t="s">
+        <v>784</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>767</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" s="2" customFormat="1" spans="1:15">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="25"/>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:15">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23" t="s">
+        <v>787</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="25"/>
+    </row>
+    <row r="22" s="4" customFormat="1" ht="15.6" spans="1:7">
+      <c r="A22" s="22" t="s">
+        <v>789</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="F22" s="39"/>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23" t="s">
+        <v>792</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>706</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>793</v>
+      </c>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="25"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>706</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="F24" s="37">
+        <v>100000</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23" t="s">
+        <v>795</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>796</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" s="2" customFormat="1" spans="1:15">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" s="2" customFormat="1" spans="1:15">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23" t="s">
+        <v>787</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" s="2" customFormat="1" spans="1:15">
+      <c r="A28" s="22" t="s">
+        <v>797</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>798</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>799</v>
+      </c>
+      <c r="F28" s="34"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" s="2" customFormat="1" spans="1:15">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23" t="s">
+        <v>800</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>801</v>
+      </c>
+      <c r="F29" s="34"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" s="2" customFormat="1" spans="1:15">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>803</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" s="2" customFormat="1" spans="1:15">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23" t="s">
+        <v>804</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>805</v>
+      </c>
+      <c r="F31" s="34"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" s="2" customFormat="1" spans="1:15">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23" t="s">
+        <v>806</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>807</v>
+      </c>
+      <c r="F32" s="34"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" s="2" customFormat="1" spans="1:15">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23" t="s">
+        <v>808</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>809</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" s="2" customFormat="1" spans="1:15">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23" t="s">
+        <v>810</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>811</v>
+      </c>
+      <c r="F34" s="34"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="25"/>
+    </row>
+    <row r="35" s="2" customFormat="1" spans="1:15">
+      <c r="A35" s="22"/>
+      <c r="B35" s="23" t="s">
+        <v>812</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>813</v>
+      </c>
+      <c r="F35" s="34"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="25"/>
+    </row>
+    <row r="36" s="2" customFormat="1" spans="1:15">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23" t="s">
+        <v>814</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>815</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="25"/>
+    </row>
+    <row r="37" s="2" customFormat="1" spans="1:15">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23" t="s">
+        <v>816</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>813</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" s="2" customFormat="1" spans="1:15">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23" t="s">
+        <v>817</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>818</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="25"/>
+    </row>
+    <row r="39" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A39" s="22" t="s">
+        <v>819</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>820</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>706</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>809</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>821</v>
+      </c>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="25"/>
+    </row>
+    <row r="40" s="2" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23" t="s">
+        <v>822</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>656</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>823</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="25"/>
+    </row>
+    <row r="41" s="2" customFormat="1" spans="1:15">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23" t="s">
+        <v>825</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>818</v>
+      </c>
+      <c r="F41" s="34"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="25"/>
+    </row>
+    <row r="42" s="2" customFormat="1" spans="1:15">
+      <c r="A42" s="22" t="s">
+        <v>826</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>827</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>828</v>
+      </c>
+      <c r="F42" s="34"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="25"/>
+    </row>
+    <row r="43" s="2" customFormat="1" spans="1:15">
+      <c r="A43" s="22"/>
+      <c r="B43" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="F43" s="34"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="25"/>
+    </row>
+    <row r="44" s="2" customFormat="1" spans="1:15">
+      <c r="A44" s="22"/>
+      <c r="B44" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>832</v>
+      </c>
+      <c r="F44" s="34"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="25"/>
+    </row>
+    <row r="45" s="2" customFormat="1" spans="1:15">
+      <c r="A45" s="22"/>
+      <c r="B45" s="23" t="s">
+        <v>833</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>834</v>
+      </c>
+      <c r="F45" s="34"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="25"/>
+    </row>
+    <row r="46" s="2" customFormat="1" spans="1:15">
+      <c r="A46" s="22"/>
+      <c r="B46" s="23" t="s">
+        <v>835</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>836</v>
+      </c>
+      <c r="F46" s="34"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="25"/>
+    </row>
+    <row r="47" s="2" customFormat="1" spans="1:15">
+      <c r="A47" s="22"/>
+      <c r="B47" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>838</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="25"/>
+    </row>
+    <row r="48" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A48" s="22" t="s">
+        <v>839</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>756</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>757</v>
+      </c>
+      <c r="F48" s="30">
+        <v>1000</v>
+      </c>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="25"/>
+    </row>
+    <row r="49" s="4" customFormat="1" ht="15.6" spans="1:15">
+      <c r="A49" s="22"/>
+      <c r="B49" s="23" t="s">
+        <v>758</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>759</v>
+      </c>
+      <c r="F49" s="30">
+        <v>2000</v>
+      </c>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="25"/>
+    </row>
+    <row r="50" s="4" customFormat="1" ht="15.6" spans="2:7">
+      <c r="B50" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="F50" s="39">
+        <v>1000</v>
+      </c>
+      <c r="G50" s="29"/>
+    </row>
+    <row r="51" s="2" customFormat="1" spans="1:15">
+      <c r="A51" s="22"/>
+      <c r="B51" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>842</v>
+      </c>
+      <c r="F51" s="41"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="25"/>
+    </row>
+    <row r="52" s="2" customFormat="1" spans="1:15">
+      <c r="A52" s="22"/>
+      <c r="B52" s="23" t="s">
+        <v>843</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="25"/>
+    </row>
+    <row r="53" s="1" customFormat="1" spans="1:15">
+      <c r="A53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="61"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="61"/>
+      <c r="O53" s="49"/>
+    </row>
+    <row r="54" s="1" customFormat="1" spans="1:15">
+      <c r="A54" s="42"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="61"/>
+      <c r="M54" s="62"/>
+      <c r="N54" s="61"/>
+      <c r="O54" s="49"/>
+    </row>
+    <row r="55" s="1" customFormat="1" spans="1:15">
+      <c r="A55" s="42"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="61"/>
+      <c r="M55" s="62"/>
+      <c r="N55" s="61"/>
+      <c r="O55" s="49"/>
+    </row>
+    <row r="56" s="1" customFormat="1" spans="1:15">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="61"/>
+      <c r="M56" s="62"/>
+      <c r="N56" s="61"/>
+      <c r="O56" s="49"/>
+    </row>
+    <row r="57" s="1" customFormat="1" spans="1:15">
+      <c r="A57" s="42"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="61"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="61"/>
+      <c r="O57" s="49"/>
+    </row>
+    <row r="58" s="1" customFormat="1" spans="1:15">
+      <c r="A58" s="42"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="61"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="61"/>
+      <c r="O58" s="49"/>
+    </row>
+    <row r="59" s="1" customFormat="1" spans="1:15">
+      <c r="A59" s="42"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="61"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="61"/>
+      <c r="O59" s="49"/>
+    </row>
+    <row r="60" s="1" customFormat="1" spans="1:15">
+      <c r="A60" s="42"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="61"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="61"/>
+      <c r="O60" s="49"/>
+    </row>
+    <row r="61" s="1" customFormat="1" spans="1:15">
+      <c r="A61" s="42"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="62"/>
+      <c r="N61" s="61"/>
+      <c r="O61" s="49"/>
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:15">
+      <c r="A62" s="42"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="62"/>
+      <c r="N62" s="61"/>
+      <c r="O62" s="49"/>
+    </row>
+    <row r="63" s="1" customFormat="1" spans="1:15">
+      <c r="A63" s="42"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="61"/>
+      <c r="M63" s="62"/>
+      <c r="N63" s="61"/>
+      <c r="O63" s="49"/>
+    </row>
+    <row r="64" s="1" customFormat="1" spans="1:15">
+      <c r="A64" s="42"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="46"/>
+      <c r="K64" s="49"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="62"/>
+      <c r="N64" s="61"/>
+      <c r="O64" s="49"/>
+    </row>
+    <row r="65" s="1" customFormat="1" spans="1:15">
+      <c r="A65" s="42"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="46"/>
+      <c r="K65" s="49"/>
+      <c r="L65" s="61"/>
+      <c r="M65" s="62"/>
+      <c r="N65" s="61"/>
+      <c r="O65" s="49"/>
+    </row>
+    <row r="66" s="1" customFormat="1" spans="1:15">
+      <c r="A66" s="42"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="61"/>
+      <c r="M66" s="62"/>
+      <c r="N66" s="61"/>
+      <c r="O66" s="49"/>
+    </row>
+    <row r="67" s="1" customFormat="1" spans="1:15">
+      <c r="A67" s="42"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="49"/>
+      <c r="L67" s="61"/>
+      <c r="M67" s="62"/>
+      <c r="N67" s="61"/>
+      <c r="O67" s="49"/>
+    </row>
+    <row r="68" s="1" customFormat="1" spans="1:15">
+      <c r="A68" s="42"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="46"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="61"/>
+      <c r="M68" s="62"/>
+      <c r="N68" s="61"/>
+      <c r="O68" s="49"/>
+    </row>
+    <row r="69" s="1" customFormat="1" spans="1:15">
+      <c r="A69" s="42"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="46"/>
+      <c r="K69" s="49"/>
+      <c r="L69" s="61"/>
+      <c r="M69" s="62"/>
+      <c r="N69" s="61"/>
+      <c r="O69" s="49"/>
+    </row>
+    <row r="70" s="1" customFormat="1" spans="1:15">
+      <c r="A70" s="42"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="45"/>
+      <c r="H70" s="45"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="46"/>
+      <c r="K70" s="49"/>
+      <c r="L70" s="61"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="61"/>
+      <c r="O70" s="49"/>
+    </row>
+    <row r="71" s="1" customFormat="1" spans="1:15">
+      <c r="A71" s="42"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="45"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="46"/>
+      <c r="K71" s="49"/>
+      <c r="L71" s="61"/>
+      <c r="M71" s="62"/>
+      <c r="N71" s="61"/>
+      <c r="O71" s="49"/>
+    </row>
+    <row r="72" s="1" customFormat="1" spans="1:15">
+      <c r="A72" s="42"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="45"/>
+      <c r="J72" s="46"/>
+      <c r="K72" s="49"/>
+      <c r="L72" s="61"/>
+      <c r="M72" s="62"/>
+      <c r="N72" s="61"/>
+      <c r="O72" s="49"/>
+    </row>
+    <row r="73" s="1" customFormat="1" spans="1:15">
+      <c r="A73" s="42"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
+      <c r="F73" s="45"/>
+      <c r="G73" s="45"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="45"/>
+      <c r="J73" s="46"/>
+      <c r="K73" s="49"/>
+      <c r="L73" s="61"/>
+      <c r="M73" s="62"/>
+      <c r="N73" s="61"/>
+      <c r="O73" s="49"/>
+    </row>
+    <row r="74" s="1" customFormat="1" spans="1:15">
+      <c r="A74" s="42"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="45"/>
+      <c r="J74" s="46"/>
+      <c r="K74" s="49"/>
+      <c r="L74" s="61"/>
+      <c r="M74" s="62"/>
+      <c r="N74" s="61"/>
+      <c r="O74" s="49"/>
+    </row>
+    <row r="75" s="1" customFormat="1" spans="1:15">
+      <c r="A75" s="42"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="45"/>
+      <c r="J75" s="46"/>
+      <c r="K75" s="49"/>
+      <c r="L75" s="61"/>
+      <c r="M75" s="62"/>
+      <c r="N75" s="61"/>
+      <c r="O75" s="49"/>
+    </row>
+    <row r="76" s="1" customFormat="1" spans="1:15">
+      <c r="A76" s="42"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="46"/>
+      <c r="K76" s="49"/>
+      <c r="L76" s="61"/>
+      <c r="M76" s="62"/>
+      <c r="N76" s="61"/>
+      <c r="O76" s="49"/>
+    </row>
+    <row r="77" s="1" customFormat="1" spans="1:15">
+      <c r="A77" s="42"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="46"/>
+      <c r="K77" s="49"/>
+      <c r="L77" s="61"/>
+      <c r="M77" s="62"/>
+      <c r="N77" s="61"/>
+      <c r="O77" s="49"/>
+    </row>
+    <row r="78" s="1" customFormat="1" spans="1:15">
+      <c r="A78" s="42"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="45"/>
+      <c r="H78" s="45"/>
+      <c r="I78" s="45"/>
+      <c r="J78" s="46"/>
+      <c r="K78" s="49"/>
+      <c r="L78" s="61"/>
+      <c r="M78" s="62"/>
+      <c r="N78" s="61"/>
+      <c r="O78" s="49"/>
+    </row>
+    <row r="79" s="1" customFormat="1" spans="1:15">
+      <c r="A79" s="42"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="45"/>
+      <c r="H79" s="45"/>
+      <c r="I79" s="45"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="49"/>
+      <c r="L79" s="61"/>
+      <c r="M79" s="62"/>
+      <c r="N79" s="61"/>
+      <c r="O79" s="49"/>
+    </row>
+    <row r="80" s="1" customFormat="1" spans="1:15">
+      <c r="A80" s="42"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="46"/>
+      <c r="K80" s="49"/>
+      <c r="L80" s="61"/>
+      <c r="M80" s="62"/>
+      <c r="N80" s="61"/>
+      <c r="O80" s="49"/>
+    </row>
+    <row r="81" s="1" customFormat="1" spans="1:15">
+      <c r="A81" s="42"/>
+      <c r="B81" s="43"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="45"/>
+      <c r="H81" s="45"/>
+      <c r="I81" s="45"/>
+      <c r="J81" s="46"/>
+      <c r="K81" s="49"/>
+      <c r="L81" s="61"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="61"/>
+      <c r="O81" s="49"/>
+    </row>
+    <row r="82" s="1" customFormat="1" spans="1:15">
+      <c r="A82" s="42"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="46"/>
+      <c r="K82" s="49"/>
+      <c r="L82" s="61"/>
+      <c r="M82" s="62"/>
+      <c r="N82" s="61"/>
+      <c r="O82" s="49"/>
+    </row>
+    <row r="83" s="6" customFormat="1" spans="1:15">
+      <c r="A83" s="63"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="65"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="66"/>
+      <c r="F83" s="66"/>
+      <c r="G83" s="66"/>
+      <c r="H83" s="66"/>
+      <c r="I83" s="66"/>
+      <c r="J83" s="67"/>
+      <c r="K83" s="68"/>
+      <c r="L83" s="69"/>
+      <c r="M83" s="70"/>
+      <c r="N83" s="69"/>
+      <c r="O83" s="68"/>
+    </row>
+    <row r="84" s="6" customFormat="1" spans="1:15">
+      <c r="A84" s="63"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="66"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="66"/>
+      <c r="J84" s="67"/>
+      <c r="K84" s="68"/>
+      <c r="L84" s="69"/>
+      <c r="M84" s="70"/>
+      <c r="N84" s="69"/>
+      <c r="O84" s="68"/>
+    </row>
+    <row r="85" s="6" customFormat="1" spans="1:15">
+      <c r="A85" s="63"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="66"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="66"/>
+      <c r="H85" s="66"/>
+      <c r="I85" s="66"/>
+      <c r="J85" s="67"/>
+      <c r="K85" s="68"/>
+      <c r="L85" s="69"/>
+      <c r="M85" s="70"/>
+      <c r="N85" s="69"/>
+      <c r="O85" s="68"/>
+    </row>
+    <row r="86" s="6" customFormat="1" spans="1:15">
+      <c r="A86" s="63"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="65"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="66"/>
+      <c r="F86" s="66"/>
+      <c r="G86" s="66"/>
+      <c r="H86" s="66"/>
+      <c r="I86" s="66"/>
+      <c r="J86" s="67"/>
+      <c r="K86" s="68"/>
+      <c r="L86" s="69"/>
+      <c r="M86" s="70"/>
+      <c r="N86" s="69"/>
+      <c r="O86" s="68"/>
+    </row>
+    <row r="87" s="6" customFormat="1" spans="1:15">
+      <c r="A87" s="63"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="65"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="66"/>
+      <c r="F87" s="66"/>
+      <c r="G87" s="66"/>
+      <c r="H87" s="66"/>
+      <c r="I87" s="66"/>
+      <c r="J87" s="67"/>
+      <c r="K87" s="68"/>
+      <c r="L87" s="69"/>
+      <c r="M87" s="70"/>
+      <c r="N87" s="69"/>
+      <c r="O87" s="68"/>
+    </row>
+    <row r="88" s="1" customFormat="1" spans="1:15">
+      <c r="A88" s="42"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="45"/>
+      <c r="I88" s="45"/>
+      <c r="J88" s="46"/>
+      <c r="K88" s="49"/>
+      <c r="L88" s="61"/>
+      <c r="M88" s="62"/>
+      <c r="N88" s="61"/>
+      <c r="O88" s="49"/>
+    </row>
+    <row r="89" s="1" customFormat="1" spans="1:15">
+      <c r="A89" s="42"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="45"/>
+      <c r="E89" s="45"/>
+      <c r="F89" s="45"/>
+      <c r="G89" s="45"/>
+      <c r="H89" s="45"/>
+      <c r="I89" s="45"/>
+      <c r="J89" s="46"/>
+      <c r="K89" s="49"/>
+      <c r="L89" s="61"/>
+      <c r="M89" s="62"/>
+      <c r="N89" s="61"/>
+      <c r="O89" s="49"/>
+    </row>
+    <row r="90" s="1" customFormat="1" spans="1:15">
+      <c r="A90" s="42"/>
+      <c r="B90" s="43"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="45"/>
+      <c r="F90" s="45"/>
+      <c r="G90" s="45"/>
+      <c r="H90" s="45"/>
+      <c r="I90" s="45"/>
+      <c r="J90" s="46"/>
+      <c r="K90" s="49"/>
+      <c r="L90" s="61"/>
+      <c r="M90" s="62"/>
+      <c r="N90" s="61"/>
+      <c r="O90" s="49"/>
+    </row>
+    <row r="91" s="1" customFormat="1" spans="1:15">
+      <c r="A91" s="42"/>
+      <c r="B91" s="43"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="45"/>
+      <c r="E91" s="45"/>
+      <c r="F91" s="45"/>
+      <c r="G91" s="45"/>
+      <c r="H91" s="45"/>
+      <c r="I91" s="45"/>
+      <c r="J91" s="46"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="61"/>
+      <c r="M91" s="62"/>
+      <c r="N91" s="61"/>
+      <c r="O91" s="49"/>
+    </row>
+    <row r="92" s="1" customFormat="1" spans="1:15">
+      <c r="A92" s="42"/>
+      <c r="B92" s="43"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="45"/>
+      <c r="F92" s="45"/>
+      <c r="G92" s="45"/>
+      <c r="H92" s="45"/>
+      <c r="I92" s="45"/>
+      <c r="J92" s="46"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="61"/>
+      <c r="M92" s="62"/>
+      <c r="N92" s="61"/>
+      <c r="O92" s="49"/>
+    </row>
+    <row r="93" s="1" customFormat="1" spans="1:15">
+      <c r="A93" s="42"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="45"/>
+      <c r="E93" s="45"/>
+      <c r="F93" s="45"/>
+      <c r="G93" s="45"/>
+      <c r="H93" s="45"/>
+      <c r="I93" s="45"/>
+      <c r="J93" s="46"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="61"/>
+      <c r="M93" s="62"/>
+      <c r="N93" s="61"/>
+      <c r="O93" s="49"/>
+    </row>
+    <row r="94" s="1" customFormat="1" spans="1:15">
+      <c r="A94" s="42"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="45"/>
+      <c r="F94" s="45"/>
+      <c r="G94" s="45"/>
+      <c r="H94" s="45"/>
+      <c r="I94" s="45"/>
+      <c r="J94" s="46"/>
+      <c r="K94" s="49"/>
+      <c r="L94" s="61"/>
+      <c r="M94" s="62"/>
+      <c r="N94" s="61"/>
+      <c r="O94" s="49"/>
+    </row>
+    <row r="95" s="1" customFormat="1" spans="1:15">
+      <c r="A95" s="42"/>
+      <c r="B95" s="43"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="45"/>
+      <c r="E95" s="45"/>
+      <c r="F95" s="45"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="45"/>
+      <c r="I95" s="45"/>
+      <c r="J95" s="46"/>
+      <c r="K95" s="49"/>
+      <c r="L95" s="61"/>
+      <c r="M95" s="62"/>
+      <c r="N95" s="61"/>
+      <c r="O95" s="49"/>
+    </row>
+    <row r="96" s="1" customFormat="1" spans="1:15">
+      <c r="A96" s="42"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="45"/>
+      <c r="F96" s="45"/>
+      <c r="G96" s="45"/>
+      <c r="H96" s="45"/>
+      <c r="I96" s="45"/>
+      <c r="J96" s="46"/>
+      <c r="K96" s="49"/>
+      <c r="L96" s="61"/>
+      <c r="M96" s="62"/>
+      <c r="N96" s="61"/>
+      <c r="O96" s="49"/>
+    </row>
+    <row r="97" s="1" customFormat="1" spans="1:15">
+      <c r="A97" s="42"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="45"/>
+      <c r="E97" s="45"/>
+      <c r="F97" s="45"/>
+      <c r="G97" s="45"/>
+      <c r="H97" s="45"/>
+      <c r="I97" s="45"/>
+      <c r="J97" s="46"/>
+      <c r="K97" s="49"/>
+      <c r="L97" s="61"/>
+      <c r="M97" s="62"/>
+      <c r="N97" s="61"/>
+      <c r="O97" s="49"/>
+    </row>
+    <row r="98" s="1" customFormat="1" spans="1:15">
+      <c r="A98" s="42"/>
+      <c r="B98" s="43"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="45"/>
+      <c r="E98" s="45"/>
+      <c r="F98" s="45"/>
+      <c r="G98" s="45"/>
+      <c r="H98" s="45"/>
+      <c r="I98" s="45"/>
+      <c r="J98" s="46"/>
+      <c r="K98" s="49"/>
+      <c r="L98" s="61"/>
+      <c r="M98" s="62"/>
+      <c r="N98" s="61"/>
+      <c r="O98" s="49"/>
+    </row>
+    <row r="99" s="1" customFormat="1" spans="1:15">
+      <c r="A99" s="42"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="45"/>
+      <c r="F99" s="45"/>
+      <c r="G99" s="45"/>
+      <c r="H99" s="45"/>
+      <c r="I99" s="45"/>
+      <c r="J99" s="46"/>
+      <c r="K99" s="49"/>
+      <c r="L99" s="61"/>
+      <c r="M99" s="62"/>
+      <c r="N99" s="61"/>
+      <c r="O99" s="49"/>
+    </row>
+    <row r="100" s="1" customFormat="1" spans="1:15">
+      <c r="A100" s="42"/>
+      <c r="B100" s="43"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="45"/>
+      <c r="E100" s="45"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="45"/>
+      <c r="I100" s="45"/>
+      <c r="J100" s="46"/>
+      <c r="K100" s="49"/>
+      <c r="L100" s="61"/>
+      <c r="M100" s="62"/>
+      <c r="N100" s="61"/>
+      <c r="O100" s="49"/>
+    </row>
+    <row r="101" s="1" customFormat="1" spans="1:15">
+      <c r="A101" s="42"/>
+      <c r="B101" s="43"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="45"/>
+      <c r="F101" s="45"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="45"/>
+      <c r="J101" s="46"/>
+      <c r="K101" s="49"/>
+      <c r="L101" s="61"/>
+      <c r="M101" s="62"/>
+      <c r="N101" s="61"/>
+      <c r="O101" s="49"/>
+    </row>
+    <row r="102" s="1" customFormat="1" spans="1:15">
+      <c r="A102" s="42"/>
+      <c r="B102" s="43"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="45"/>
+      <c r="E102" s="45"/>
+      <c r="F102" s="45"/>
+      <c r="G102" s="45"/>
+      <c r="H102" s="45"/>
+      <c r="I102" s="45"/>
+      <c r="J102" s="46"/>
+      <c r="K102" s="49"/>
+      <c r="L102" s="61"/>
+      <c r="M102" s="62"/>
+      <c r="N102" s="61"/>
+      <c r="O102" s="49"/>
+    </row>
+    <row r="103" s="1" customFormat="1" spans="1:15">
+      <c r="A103" s="42"/>
+      <c r="B103" s="43"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="45"/>
+      <c r="E103" s="45"/>
+      <c r="F103" s="45"/>
+      <c r="G103" s="45"/>
+      <c r="H103" s="45"/>
+      <c r="I103" s="45"/>
+      <c r="J103" s="46"/>
+      <c r="K103" s="49"/>
+      <c r="L103" s="61"/>
+      <c r="M103" s="62"/>
+      <c r="N103" s="61"/>
+      <c r="O103" s="49"/>
+    </row>
+    <row r="104" s="1" customFormat="1" spans="1:15">
+      <c r="A104" s="42"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="45"/>
+      <c r="E104" s="45"/>
+      <c r="F104" s="45"/>
+      <c r="G104" s="45"/>
+      <c r="H104" s="45"/>
+      <c r="I104" s="45"/>
+      <c r="J104" s="46"/>
+      <c r="K104" s="49"/>
+      <c r="L104" s="61"/>
+      <c r="M104" s="62"/>
+      <c r="N104" s="61"/>
+      <c r="O104" s="49"/>
+    </row>
+    <row r="105" s="1" customFormat="1" spans="1:15">
+      <c r="A105" s="42"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="45"/>
+      <c r="E105" s="45"/>
+      <c r="F105" s="45"/>
+      <c r="G105" s="45"/>
+      <c r="H105" s="45"/>
+      <c r="I105" s="45"/>
+      <c r="J105" s="46"/>
+      <c r="K105" s="49"/>
+      <c r="L105" s="61"/>
+      <c r="M105" s="62"/>
+      <c r="N105" s="61"/>
+      <c r="O105" s="49"/>
+    </row>
+    <row r="106" s="1" customFormat="1" spans="1:15">
+      <c r="A106" s="42"/>
+      <c r="B106" s="43"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="45"/>
+      <c r="F106" s="45"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="45"/>
+      <c r="I106" s="45"/>
+      <c r="J106" s="46"/>
+      <c r="K106" s="49"/>
+      <c r="L106" s="61"/>
+      <c r="M106" s="62"/>
+      <c r="N106" s="61"/>
+      <c r="O106" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N1">
+    <cfRule type="beginsWith" dxfId="2" priority="60" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="59" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="58" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18">
+    <cfRule type="beginsWith" dxfId="2" priority="45" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N18,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="44" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N18,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="43" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N18,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N24">
+    <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N24,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N24,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N24,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
+    <cfRule type="beginsWith" dxfId="2" priority="39" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N26,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="38" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N26,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="37" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N26,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N27">
+    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N27,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N27,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N27,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
+    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N33,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N33,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N33,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41">
+    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N41,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N41,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="34" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N41,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N64">
+    <cfRule type="beginsWith" dxfId="2" priority="21" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N64,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N64,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="19" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N64,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N4">
+    <cfRule type="beginsWith" dxfId="2" priority="54" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N3,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="53" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N3,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="52" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N3,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:N10">
+    <cfRule type="beginsWith" dxfId="2" priority="51" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N5,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="50" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N5,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="49" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N5,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:N12">
+    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N11,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="47" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N11,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="46" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N11,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13:N17">
+    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N13,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N13,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="40" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N13,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20:N23">
+    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N20,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N20,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N20,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N32">
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N29,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N29,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N29,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N53:N54">
+    <cfRule type="beginsWith" dxfId="2" priority="33" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N53,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="32" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N53,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="31" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N53,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N55:N56">
+    <cfRule type="beginsWith" dxfId="2" priority="30" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N55,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="29" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N55,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="28" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N55,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N57:N61">
+    <cfRule type="beginsWith" dxfId="2" priority="27" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N57,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="26" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N57,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="25" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N57,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N76:N78">
+    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N76,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N76,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N76,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N34:N40 N42:N52 N79:N106 N67:N75">
+    <cfRule type="beginsWith" dxfId="2" priority="57" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N34,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="56" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N34,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="55" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N34,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N62:N63 N65:N66">
+    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N62,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N62,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N62,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C20 C23 C26 C27 C29 C32 C45 C46 C47 C54 C57 C60 C61 C64 C65 C66 C67 C70 C71 C72 C73 C76 C79 C80 C81 C82 C13:C14 C15:C19 C21:C22 C30:C31 C34:C35 C36:C44 C48:C53 C55:C56 C58:C59 C62:C63 C68:C69 C74:C75 C77:C78 C83:C106">
+      <formula1>target</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D15 D18 D19 D20 D21 D22 D23 D26 D27 D29 D30 D31 D32 D45 D46 D47 D54 D57 D60 D61 D64 D65 D66 D67 D70 D71 D72 D73 D76 D79 D80 D81 D82 D13:D14 D16:D17 D34:D35 D36:D44 D48:D53 D55:D56 D58:D59 D62:D63 D68:D69 D74:D75 D77:D78 D83:D106">
+      <formula1>INDIRECT(C5)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>